<commit_message>
update to LFM 2022 datafile
Adding in the three missing dry weights, and creating final csv for analysis
</commit_message>
<xml_diff>
--- a/2022/LFM_June_2022/PWD_Jun2022_LFM_WP_RawData_Prep.xlsx
+++ b/2022/LFM_June_2022/PWD_Jun2022_LFM_WP_RawData_Prep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinakozanitas/GitHub/PepperwoodVegPlots/2022/LFM_June_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ADDDF9-56AF-FB41-B94A-DD05E37AC9B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A594DF1-3104-B541-A437-6B5EFD1B6C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="2460" windowWidth="28240" windowHeight="15480" activeTab="2" xr2:uid="{05CBDBC3-C58E-254F-9CCB-F423A62E9A36}"/>
+    <workbookView xWindow="1280" yWindow="1740" windowWidth="28240" windowHeight="15480" activeTab="2" xr2:uid="{05CBDBC3-C58E-254F-9CCB-F423A62E9A36}"/>
   </bookViews>
   <sheets>
     <sheet name="WP_LFM_RAW" sheetId="2" r:id="rId1"/>
@@ -649,9 +649,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBB63F9D-A779-474A-9790-68A1B1C3510F}">
   <dimension ref="A1:AJ82"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="116" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG2" sqref="AG2:AI69"/>
+    <sheetView topLeftCell="U1" zoomScale="116" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK21" sqref="AK21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2579,6 +2579,9 @@
       <c r="AD23" s="1">
         <v>64.88</v>
       </c>
+      <c r="AE23" s="1">
+        <v>51.01</v>
+      </c>
       <c r="AF23" s="1" t="s">
         <v>37</v>
       </c>
@@ -2586,6 +2589,18 @@
         <f t="shared" si="2"/>
         <v>27.83</v>
       </c>
+      <c r="AH23" s="1">
+        <f t="shared" si="3"/>
+        <v>13.96</v>
+      </c>
+      <c r="AI23" s="1">
+        <f t="shared" si="4"/>
+        <v>13.869999999999997</v>
+      </c>
+      <c r="AJ23" s="1">
+        <f t="shared" si="5"/>
+        <v>0.99355300859598827</v>
+      </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -3550,17 +3565,32 @@
         <v>0.36</v>
       </c>
       <c r="AC34" s="1">
-        <v>37.090000000000003</v>
+        <v>37.19</v>
       </c>
       <c r="AD34" s="1">
-        <v>44.67</v>
+        <v>49.83</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>42.34</v>
       </c>
       <c r="AF34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AG34" s="1">
-        <f t="shared" si="2"/>
-        <v>7.5799999999999983</v>
+        <f>(AD34-AC34)</f>
+        <v>12.64</v>
+      </c>
+      <c r="AH34" s="1">
+        <f>(AE34-AC34)</f>
+        <v>5.1500000000000057</v>
+      </c>
+      <c r="AI34" s="1">
+        <f>(AG34-AH34)</f>
+        <v>7.4899999999999949</v>
+      </c>
+      <c r="AJ34" s="1">
+        <f>(AI34/AH34)</f>
+        <v>1.4543689320388324</v>
       </c>
     </row>
     <row r="35" spans="1:36" x14ac:dyDescent="0.2">
@@ -4326,17 +4356,32 @@
         <v>0.38900000000000001</v>
       </c>
       <c r="AC43" s="1">
-        <v>37.19</v>
+        <v>37.090000000000003</v>
       </c>
       <c r="AD43" s="1">
-        <v>49.83</v>
+        <v>44.67</v>
+      </c>
+      <c r="AE43" s="1">
+        <v>40.81</v>
       </c>
       <c r="AF43" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AG43" s="1">
-        <f t="shared" si="2"/>
-        <v>12.64</v>
+        <f>(AD43-AC43)</f>
+        <v>7.5799999999999983</v>
+      </c>
+      <c r="AH43" s="1">
+        <f>(AE43-AC43)</f>
+        <v>3.7199999999999989</v>
+      </c>
+      <c r="AI43" s="1">
+        <f>(AG43-AH43)</f>
+        <v>3.8599999999999994</v>
+      </c>
+      <c r="AJ43" s="1">
+        <f>(AI43/AH43)</f>
+        <v>1.0376344086021507</v>
       </c>
     </row>
     <row r="44" spans="1:36" x14ac:dyDescent="0.2">
@@ -7522,8 +7567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F26387-5A2C-7249-9418-13E670B128BC}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8323,8 +8368,12 @@
       <c r="J23" s="1">
         <v>27.83</v>
       </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
+      <c r="K23" s="1">
+        <v>13.96</v>
+      </c>
+      <c r="L23" s="1">
+        <v>13.869999999999997</v>
+      </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -8724,13 +8773,15 @@
         <v>0.28166666666666668</v>
       </c>
       <c r="J34" s="1">
-        <v>7.5799999999999983</v>
-      </c>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
+        <v>12.64</v>
+      </c>
+      <c r="K34" s="1">
+        <v>5.1500000000000057</v>
+      </c>
+      <c r="L34" s="1">
+        <v>7.4899999999999949</v>
+      </c>
       <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -9051,10 +9102,14 @@
         <v>1.7066666666666668</v>
       </c>
       <c r="J43" s="1">
-        <v>12.64</v>
-      </c>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+        <v>7.5799999999999983</v>
+      </c>
+      <c r="K43" s="1">
+        <v>3.7199999999999989</v>
+      </c>
+      <c r="L43" s="1">
+        <v>3.8599999999999994</v>
+      </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>

</xml_diff>